<commit_message>
Added work in progress climate model added
</commit_message>
<xml_diff>
--- a/Modelling.xlsx
+++ b/Modelling.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Infrared Transparency" sheetId="1" r:id="rId1"/>
+    <sheet name="Albedo" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>Albedo</t>
   </si>
@@ -150,6 +151,24 @@
   </si>
   <si>
     <t>Water Fraction</t>
+  </si>
+  <si>
+    <t>ocean</t>
+  </si>
+  <si>
+    <t>land</t>
+  </si>
+  <si>
+    <t>ice</t>
+  </si>
+  <si>
+    <t>cloud</t>
+  </si>
+  <si>
+    <t>dry land</t>
+  </si>
+  <si>
+    <t>liquid water</t>
   </si>
 </sst>
 </file>
@@ -232,7 +251,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -253,6 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -261,6 +281,9 @@
   </cellStyles>
   <dxfs count="29">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="166" formatCode="0.000000"/>
     </dxf>
     <dxf>
@@ -328,9 +351,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -488,7 +508,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$AE$2:$AE$6</c:f>
+              <c:f>'Infrared Transparency'!$AE$2:$AE$6</c:f>
               <c:numCache>
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -509,7 +529,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AF$2:$AF$6</c:f>
+              <c:f>'Infrared Transparency'!$AF$2:$AF$6</c:f>
               <c:numCache>
                 <c:formatCode>0.000000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -538,11 +558,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="633531544"/>
-        <c:axId val="518123248"/>
+        <c:axId val="213163280"/>
+        <c:axId val="213145448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="633531544"/>
+        <c:axId val="213163280"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -600,12 +620,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="518123248"/>
+        <c:crossAx val="213145448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="518123248"/>
+        <c:axId val="213145448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -663,7 +683,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="633531544"/>
+        <c:crossAx val="213163280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1324,53 +1344,53 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="I1:AI5" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="I1:AI5" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="I1:AI5"/>
   <tableColumns count="27">
     <tableColumn id="7" name="Planet"/>
     <tableColumn id="1" name="Albedo"/>
-    <tableColumn id="2" name="Greenhouse Fraction" dataDxfId="22">
+    <tableColumn id="2" name="Greenhouse Fraction" dataDxfId="23">
       <calculatedColumnFormula>1-C5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Inverse" dataDxfId="21">
+    <tableColumn id="15" name="Inverse" dataDxfId="22">
       <calculatedColumnFormula>1/(1-Table2[[#This Row],[Greenhouse Fraction]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" name="Emissivity"/>
-    <tableColumn id="4" name="Flux Density" dataDxfId="20"/>
-    <tableColumn id="5" name="Avg Flux Density" dataDxfId="19">
+    <tableColumn id="4" name="Flux Density" dataDxfId="21"/>
+    <tableColumn id="5" name="Avg Flux Density" dataDxfId="20">
       <calculatedColumnFormula>Table2[Flux Density]*0.25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" name="Water Fraction" dataDxfId="18"/>
-    <tableColumn id="6" name="Temperature" dataDxfId="17">
+    <tableColumn id="28" name="Water Fraction" dataDxfId="19"/>
+    <tableColumn id="6" name="Temperature" dataDxfId="18">
       <calculatedColumnFormula>POWER((1-Table2[Albedo])*Table2[[#This Row],[Avg Flux Density]]/(1-Table2[Greenhouse Fraction])/0.00000005670374/Table2[Emissivity],0.25)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Gravity"/>
-    <tableColumn id="9" name="atm_CO2" dataDxfId="16"/>
-    <tableColumn id="11" name="atm_H2O" dataDxfId="15">
+    <tableColumn id="9" name="atm_CO2" dataDxfId="17"/>
+    <tableColumn id="11" name="atm_H2O" dataDxfId="16">
       <calculatedColumnFormula>0.004</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="atm_N2O" dataDxfId="14"/>
-    <tableColumn id="27" name="atm_O3" dataDxfId="13"/>
-    <tableColumn id="14" name="Pressure" dataDxfId="12"/>
-    <tableColumn id="10" name="n_CO2" dataDxfId="11">
+    <tableColumn id="26" name="atm_N2O" dataDxfId="15"/>
+    <tableColumn id="27" name="atm_O3" dataDxfId="14"/>
+    <tableColumn id="14" name="Pressure" dataDxfId="13"/>
+    <tableColumn id="10" name="n_CO2" dataDxfId="12">
       <calculatedColumnFormula>Table2[[#This Row],[atm_CO2]]/Table2[[#This Row],[Gravity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="n_CH4" dataDxfId="10">
+    <tableColumn id="12" name="n_CH4" dataDxfId="11">
       <calculatedColumnFormula>1.7*0.000001</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="n_H2O" dataDxfId="9">
+    <tableColumn id="13" name="n_H2O" dataDxfId="10">
       <calculatedColumnFormula>Table2[[#This Row],[atm_H2O]]/Table2[[#This Row],[Gravity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="n_N20" dataDxfId="8">
+    <tableColumn id="24" name="n_N20" dataDxfId="9">
       <calculatedColumnFormula>Table2[[#This Row],[atm_N2O]]/Table2[[#This Row],[Gravity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="n_O3" dataDxfId="7">
+    <tableColumn id="25" name="n_O3" dataDxfId="8">
       <calculatedColumnFormula>Table2[[#This Row],[atm_O3]]/Table2[[#This Row],[Gravity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="CO2_e" dataDxfId="6">
+    <tableColumn id="16" name="CO2_e" dataDxfId="7">
       <calculatedColumnFormula>Table2[[#This Row],[n_CO2]]+Table2[[#This Row],[n_CH4]]*$AL$3+Table2[[#This Row],[n_H2O]]*$AL$4+Table2[[#This Row],[n_N20]]*$AL$5+Table2[[#This Row],[n_O3]]*$AL$6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="Pressure Factor" dataDxfId="0">
+    <tableColumn id="18" name="Pressure Factor" dataDxfId="6">
       <calculatedColumnFormula>POWER(Table2[[#This Row],[Pressure]],2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="19" name="Greenhouse Effect" dataDxfId="5">
@@ -1394,7 +1414,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="AK1:AN6" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="AK1:AN6" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="AK1:AN6"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Gas"/>
@@ -1671,7 +1691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="AI3" sqref="AI3"/>
     </sheetView>
   </sheetViews>
@@ -2455,4 +2475,112 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="14">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="14">
+        <f>1-B1</f>
+        <v>0.29200000000000004</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="14">
+        <v>0.51</v>
+      </c>
+      <c r="C3" s="14">
+        <f>B3</f>
+        <v>0.51</v>
+      </c>
+      <c r="D3" s="14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="14">
+        <f>0.1*B2</f>
+        <v>2.9200000000000004E-2</v>
+      </c>
+      <c r="C4" s="14">
+        <f>B4*(1-$B$3)</f>
+        <v>1.4308000000000001E-2</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="14">
+        <f>B2-B4/2</f>
+        <v>0.27740000000000004</v>
+      </c>
+      <c r="C5" s="14">
+        <f>B5*(1-$B$3)</f>
+        <v>0.13592600000000002</v>
+      </c>
+      <c r="D5" s="14">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="14">
+        <f>B1-B4/2</f>
+        <v>0.69340000000000002</v>
+      </c>
+      <c r="C6" s="14">
+        <f>B6*(1-$B$3)</f>
+        <v>0.33976600000000001</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14">
+        <f>D6*C6+D5*C5+D3*C3+D4*C4</f>
+        <v>0.30486044000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>